<commit_message>
second commit - testng
</commit_message>
<xml_diff>
--- a/PC_Account_Create/src/main/java/excelFile/PolicyAccount.xlsx
+++ b/PC_Account_Create/src/main/java/excelFile/PolicyAccount.xlsx
@@ -419,7 +419,7 @@
     <t>No - New Driver</t>
   </si>
   <si>
-    <t>1/23/2025</t>
+    <t>1/23/2021</t>
   </si>
   <si>
     <t>1/18/1993</t>
@@ -1964,7 +1964,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>

</xml_diff>

<commit_message>
Third commit - multibrowser config fix
</commit_message>
<xml_diff>
--- a/PC_Account_Create/src/main/java/excelFile/PolicyAccount.xlsx
+++ b/PC_Account_Create/src/main/java/excelFile/PolicyAccount.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="137">
   <si>
     <t>Company Name</t>
   </si>
@@ -119,10 +119,10 @@
     <t>7126736458</t>
   </si>
   <si>
-    <t>Macus</t>
-  </si>
-  <si>
-    <t>Hale</t>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Hood</t>
   </si>
   <si>
     <t>6423683145</t>
@@ -167,7 +167,7 @@
     <t>5424749837</t>
   </si>
   <si>
-    <t>Robert</t>
+    <t>James</t>
   </si>
   <si>
     <t>Albert</t>
@@ -419,7 +419,7 @@
     <t>No - New Driver</t>
   </si>
   <si>
-    <t>1/23/2021</t>
+    <t>1/23/2025</t>
   </si>
   <si>
     <t>1/18/1993</t>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>33000</t>
+  </si>
+  <si>
+    <t>9032555138</t>
   </si>
 </sst>
 </file>
@@ -1400,8 +1403,8 @@
   <sheetPr/>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6"/>
@@ -1961,13 +1964,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="15.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="22.7142857142857" customWidth="1"/>
@@ -2085,6 +2088,56 @@
         <v>135</v>
       </c>
     </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>